<commit_message>
added simple mite map examples and ran a few examples to create stuff we can show at the workshop
</commit_message>
<xml_diff>
--- a/data_in/Complete Mite Monitor GP.xlsx
+++ b/data_in/Complete Mite Monitor GP.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GPetersen\Desktop\Mite_Monitor\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E77676D-7377-478E-9E35-85216BFF2103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62DA990-E512-4EA6-A09E-35F4258DC25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-3435" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{16EEC1AB-7B5A-40BF-9CB7-5EB9EEF202EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{16EEC1AB-7B5A-40BF-9CB7-5EB9EEF202EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Mite Counts" sheetId="1" r:id="rId1"/>
     <sheet name="Apiaries" sheetId="5" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Apiaries!$A$1:$D$178</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Mite Counts'!$A$1:$H$426</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2196" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="551">
   <si>
     <t xml:space="preserve">TREATMENT
 </t>
@@ -919,9 +923,6 @@
     <t>-43.843432</t>
   </si>
   <si>
-    <t>71.8411171</t>
-  </si>
-  <si>
     <t>-43.82891</t>
   </si>
   <si>
@@ -949,9 +950,6 @@
     <t>-43.7006</t>
   </si>
   <si>
-    <t>71.76235</t>
-  </si>
-  <si>
     <t>-43.81164</t>
   </si>
   <si>
@@ -979,9 +977,6 @@
     <t>-43.683</t>
   </si>
   <si>
-    <t>1.61459</t>
-  </si>
-  <si>
     <t>-43.93835</t>
   </si>
   <si>
@@ -1159,9 +1154,6 @@
     <t>-43.99842</t>
   </si>
   <si>
-    <t>42, 171.6</t>
-  </si>
-  <si>
     <t>-43.57168</t>
   </si>
   <si>
@@ -1195,9 +1187,6 @@
     <t>-43.6438</t>
   </si>
   <si>
-    <t>71.41188</t>
-  </si>
-  <si>
     <t>-43.63885</t>
   </si>
   <si>
@@ -1282,9 +1271,6 @@
     <t>-44.0373</t>
   </si>
   <si>
-    <t>71.67817</t>
-  </si>
-  <si>
     <t>-44.03179</t>
   </si>
   <si>
@@ -1294,9 +1280,6 @@
     <t>-44.0947</t>
   </si>
   <si>
-    <t>71.62901</t>
-  </si>
-  <si>
     <t>-43.89347</t>
   </si>
   <si>
@@ -1336,9 +1319,6 @@
     <t>-43.666</t>
   </si>
   <si>
-    <t>1.53644</t>
-  </si>
-  <si>
     <t>-43.9381995</t>
   </si>
   <si>
@@ -1396,9 +1376,6 @@
     <t>-43.7759</t>
   </si>
   <si>
-    <t>71.70094</t>
-  </si>
-  <si>
     <t>-44.0044491</t>
   </si>
   <si>
@@ -1414,9 +1391,6 @@
     <t>-43.756131</t>
   </si>
   <si>
-    <t>71.9865817</t>
-  </si>
-  <si>
     <t>-43.82791</t>
   </si>
   <si>
@@ -1492,9 +1466,6 @@
     <t>-43.847</t>
   </si>
   <si>
-    <t>2.10013</t>
-  </si>
-  <si>
     <t>-43.51673</t>
   </si>
   <si>
@@ -1546,9 +1517,6 @@
     <t>-43.7081</t>
   </si>
   <si>
-    <t>71.72697</t>
-  </si>
-  <si>
     <t>-43.69794</t>
   </si>
   <si>
@@ -1556,9 +1524,6 @@
   </si>
   <si>
     <t>-43.858</t>
-  </si>
-  <si>
-    <t>1.93371</t>
   </si>
   <si>
     <t>-43.8137538</t>
@@ -2167,9 +2132,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C50DC2-CA37-49EF-A0FD-69B4D39A71AD}">
   <dimension ref="A1:H618"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A601" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A428" sqref="A428:A618"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C357" sqref="C357:C360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8681,7 +8646,7 @@
         <v>47</v>
       </c>
       <c r="C356" s="19">
-        <v>36878</v>
+        <v>44183</v>
       </c>
       <c r="D356" s="3">
         <v>1</v>
@@ -8698,7 +8663,7 @@
         <v>47</v>
       </c>
       <c r="C357" s="19">
-        <v>36878</v>
+        <v>44183</v>
       </c>
       <c r="D357" s="3">
         <v>2</v>
@@ -8715,7 +8680,7 @@
         <v>47</v>
       </c>
       <c r="C358" s="19">
-        <v>36878</v>
+        <v>44183</v>
       </c>
       <c r="D358" s="3">
         <v>3</v>
@@ -8732,7 +8697,7 @@
         <v>47</v>
       </c>
       <c r="C359" s="19">
-        <v>36878</v>
+        <v>44183</v>
       </c>
       <c r="D359" s="3">
         <v>5</v>
@@ -8749,7 +8714,7 @@
         <v>47</v>
       </c>
       <c r="C360" s="19">
-        <v>36878</v>
+        <v>44183</v>
       </c>
       <c r="D360" s="3">
         <v>6</v>
@@ -9879,1542 +9844,583 @@
       </c>
     </row>
     <row r="427" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A427" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B427" s="14" t="s">
-        <v>107</v>
-      </c>
+      <c r="A427" s="14"/>
     </row>
     <row r="428" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A428" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B428" s="14" t="s">
-        <v>108</v>
-      </c>
+      <c r="A428" s="14"/>
     </row>
     <row r="429" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A429" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B429" s="14" t="s">
-        <v>109</v>
-      </c>
+      <c r="A429" s="14"/>
     </row>
     <row r="430" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A430" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B430" s="14" t="s">
-        <v>110</v>
-      </c>
+      <c r="A430" s="14"/>
     </row>
     <row r="431" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A431" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B431" s="14" t="s">
-        <v>110</v>
-      </c>
+      <c r="A431" s="14"/>
     </row>
     <row r="432" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A432" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B432" s="14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A433" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B433" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A434" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B434" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A435" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B435" s="14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A436" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B436" s="14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A437" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B437" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A438" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B438" s="14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A439" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B439" s="14" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A440" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B440" s="14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A441" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B441" s="14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A442" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B442" s="14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A443" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B443" s="14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A444" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B444" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A445" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B445" s="14" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A446" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B446" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A447" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B447" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A448" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B448" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A449" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B449" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A450" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B450" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A451" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B451" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A452" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B452" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A453" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B453" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A454" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B454" s="14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A455" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B455" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A456" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B456" s="14" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A457" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B457" s="14" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A458" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B458" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A459" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B459" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A460" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B460" s="14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A461" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B461" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A462" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B462" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A463" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B463" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A464" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B464" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="465" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A465" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B465" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="466" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A466" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B466" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A467" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B467" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A468" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B468" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A469" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B469" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A470" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B470" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A471" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B471" s="14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A472" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B472" s="14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A473" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B473" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A474" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B474" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A475" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B475" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A476" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B476" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A477" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B477" s="14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A478" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B478" s="14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A479" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B479" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A480" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B480" s="14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="481" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A481" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B481" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="482" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A482" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B482" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A483" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B483" s="14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="484" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A484" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B484" s="14" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="485" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A485" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B485" s="14" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="486" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A486" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B486" s="14" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="487" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A487" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B487" s="14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="488" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A488" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B488" s="14" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="489" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A489" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B489" s="14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="490" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A490" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B490" s="14" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="491" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A491" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B491" s="14" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="492" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A492" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B492" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="493" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A493" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B493" s="14" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="494" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A494" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B494" s="14" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="495" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A495" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B495" s="14" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="496" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A496" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B496" s="14" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A497" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B497" s="14" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="498" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A498" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B498" s="14" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="499" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A499" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B499" s="14" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="500" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A500" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B500" s="14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="501" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A501" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B501" s="14" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="502" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A502" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B502" s="14" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="503" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A503" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B503" s="14" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="504" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A504" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B504" s="14" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="505" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A505" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B505" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="506" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A506" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B506" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="507" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A507" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B507" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="508" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A508" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B508" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="509" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A509" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B509" s="14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="510" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A510" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B510" s="14" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="511" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A511" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B511" s="14" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="512" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A512" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B512" s="14" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="513" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A513" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B513" s="14" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="514" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A514" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B514" s="14" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="515" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A515" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B515" s="14" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="516" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A516" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B516" s="14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="517" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A517" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B517" s="14" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="518" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A518" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B518" s="14" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="519" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A519" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B519" s="14" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="520" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A520" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B520" s="14" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="521" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A521" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B521" s="14" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="522" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A522" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B522" s="14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="523" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A523" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B523" s="14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="524" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A524" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B524" s="14" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="525" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A525" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B525" s="14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="526" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A526" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B526" s="14" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="527" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A527" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B527" s="14" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="528" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A528" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B528" s="14" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="529" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A529" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B529" s="14" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="530" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A530" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B530" s="14" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="531" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A531" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B531" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="532" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A532" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B532" s="14" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="533" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A533" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B533" s="14" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="534" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A534" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B534" s="14" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="535" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A535" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B535" s="14" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="536" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A536" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B536" s="14" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="537" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A537" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B537" s="14" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="538" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A538" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B538" s="14" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="539" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A539" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B539" s="14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="540" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A540" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B540" s="14" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="541" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A541" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B541" s="14" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="542" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A542" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B542" s="14" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="543" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A543" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B543" s="14" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="544" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A544" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B544" s="14" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="545" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A545" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B545" s="14" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="546" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A546" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B546" s="14" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="547" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A547" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B547" s="14" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="548" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A548" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B548" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="549" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A549" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B549" s="14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="550" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A550" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B550" s="14" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="551" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A551" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B551" s="14" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="552" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A552" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B552" s="14" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="553" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A553" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B553" s="14" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="554" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A554" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B554" s="14" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="555" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A555" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B555" s="14" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="556" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A556" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B556" s="14" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="557" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A557" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B557" s="14" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="558" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A558" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B558" s="14" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="559" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A559" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B559" s="14" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="560" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A560" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B560" s="14" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="561" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A561" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B561" s="14" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="562" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A562" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B562" s="14" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="563" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A563" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B563" s="14" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="564" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A564" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B564" s="14" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="565" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A565" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B565" s="14" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="566" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A566" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B566" s="14" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="567" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A567" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B567" s="14" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="568" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A568" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B568" s="14" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="569" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A569" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B569" s="14" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="570" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A570" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B570" s="14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="571" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A571" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B571" s="14" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="572" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A572" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B572" s="14" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="573" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A573" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B573" s="14" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="574" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A574" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B574" s="14" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="575" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A575" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B575" s="14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="576" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A576" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B576" s="14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="577" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A577" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B577" s="14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="578" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A578" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B578" s="14" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="579" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A579" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B579" s="14" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="580" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A580" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B580" s="14" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="581" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A581" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B581" s="14" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="582" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A582" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B582" s="14" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="583" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A583" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B583" s="14" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="584" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A584" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B584" s="14" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="585" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A585" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B585" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="586" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A586" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B586" s="14" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="587" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A587" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B587" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="588" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A588" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B588" s="14" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="589" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A589" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B589" s="14" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="590" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A590" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B590" s="14" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="591" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A591" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B591" s="14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="592" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A592" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B592" s="14" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="593" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A593" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B593" s="14" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="594" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A594" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B594" s="14" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="595" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A595" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B595" s="14" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="596" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A596" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B596" s="14" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="597" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A597" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B597" s="14" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="598" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A598" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B598" s="14" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="599" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A599" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B599" s="14" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="600" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A600" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B600" s="14" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="601" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A601" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B601" s="14" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="602" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A602" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B602" s="14" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="603" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A603" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B603" s="14" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="604" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A604" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B604" s="14" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="605" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A605" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B605" s="14" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="606" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A606" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B606" s="14" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="607" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A607" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B607" s="14" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="608" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A608" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B608" s="14" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="609" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A609" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B609" s="14" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="610" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A610" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B610" s="14" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="611" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A611" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B611" s="14" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="612" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A612" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B612" s="14" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="613" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A613" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B613" s="14" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="614" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A614" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B614" s="14" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="615" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A615" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B615" s="14" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="616" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A616" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B616" s="14" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="617" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A617" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B617" s="14" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="618" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A618" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B618" s="14" t="s">
-        <v>260</v>
-      </c>
+      <c r="A432" s="14"/>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" s="14"/>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434" s="14"/>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435" s="14"/>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" s="14"/>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437" s="14"/>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438" s="14"/>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" s="14"/>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" s="14"/>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" s="14"/>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" s="14"/>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" s="14"/>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" s="14"/>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" s="14"/>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" s="14"/>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" s="14"/>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" s="14"/>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" s="14"/>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" s="14"/>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" s="14"/>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" s="14"/>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453" s="14"/>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" s="14"/>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" s="14"/>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" s="14"/>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457" s="14"/>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A458" s="14"/>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A459" s="14"/>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460" s="14"/>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461" s="14"/>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462" s="14"/>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463" s="14"/>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" s="14"/>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" s="14"/>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" s="14"/>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" s="14"/>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" s="14"/>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" s="14"/>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" s="14"/>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" s="14"/>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" s="14"/>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" s="14"/>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" s="14"/>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" s="14"/>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" s="14"/>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" s="14"/>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" s="14"/>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" s="14"/>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" s="14"/>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" s="14"/>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" s="14"/>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A483" s="14"/>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A484" s="14"/>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A485" s="14"/>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A486" s="14"/>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A487" s="14"/>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A488" s="14"/>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A489" s="14"/>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A490" s="14"/>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A491" s="14"/>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A492" s="14"/>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A493" s="14"/>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A494" s="14"/>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A495" s="14"/>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A496" s="14"/>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A497" s="14"/>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A498" s="14"/>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A499" s="14"/>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500" s="14"/>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501" s="14"/>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A502" s="14"/>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A503" s="14"/>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A504" s="14"/>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A505" s="14"/>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A506" s="14"/>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A507" s="14"/>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A508" s="14"/>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A509" s="14"/>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A510" s="14"/>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511" s="14"/>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A512" s="14"/>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A513" s="14"/>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514" s="14"/>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515" s="14"/>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A516" s="14"/>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A517" s="14"/>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A518" s="14"/>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A519" s="14"/>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A520" s="14"/>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A521" s="14"/>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522" s="14"/>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523" s="14"/>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524" s="14"/>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A525" s="14"/>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A526" s="14"/>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A527" s="14"/>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A528" s="14"/>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A529" s="14"/>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A530" s="14"/>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A531" s="14"/>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A532" s="14"/>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A533" s="14"/>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A534" s="14"/>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A535" s="14"/>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A536" s="14"/>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A537" s="14"/>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A538" s="14"/>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A539" s="14"/>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A540" s="14"/>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A541" s="14"/>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A542" s="14"/>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A543" s="14"/>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A544" s="14"/>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A545" s="14"/>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A546" s="14"/>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A547" s="14"/>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A548" s="14"/>
+    </row>
+    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A549" s="14"/>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A550" s="14"/>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A551" s="14"/>
+    </row>
+    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A552" s="14"/>
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A553" s="14"/>
+    </row>
+    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A554" s="14"/>
+    </row>
+    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A555" s="14"/>
+    </row>
+    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A556" s="14"/>
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A557" s="14"/>
+    </row>
+    <row r="558" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A558" s="14"/>
+    </row>
+    <row r="559" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A559" s="14"/>
+    </row>
+    <row r="560" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A560" s="14"/>
+    </row>
+    <row r="561" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A561" s="14"/>
+    </row>
+    <row r="562" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A562" s="14"/>
+    </row>
+    <row r="563" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A563" s="14"/>
+    </row>
+    <row r="564" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A564" s="14"/>
+    </row>
+    <row r="565" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A565" s="14"/>
+    </row>
+    <row r="566" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A566" s="14"/>
+    </row>
+    <row r="567" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A567" s="14"/>
+    </row>
+    <row r="568" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A568" s="14"/>
+    </row>
+    <row r="569" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A569" s="14"/>
+    </row>
+    <row r="570" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A570" s="14"/>
+    </row>
+    <row r="571" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A571" s="14"/>
+    </row>
+    <row r="572" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A572" s="14"/>
+    </row>
+    <row r="573" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A573" s="14"/>
+    </row>
+    <row r="574" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A574" s="14"/>
+    </row>
+    <row r="575" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A575" s="14"/>
+    </row>
+    <row r="576" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A576" s="14"/>
+    </row>
+    <row r="577" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A577" s="14"/>
+    </row>
+    <row r="578" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A578" s="14"/>
+    </row>
+    <row r="579" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A579" s="14"/>
+    </row>
+    <row r="580" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A580" s="14"/>
+    </row>
+    <row r="581" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A581" s="14"/>
+    </row>
+    <row r="582" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A582" s="14"/>
+    </row>
+    <row r="583" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A583" s="14"/>
+    </row>
+    <row r="584" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A584" s="14"/>
+    </row>
+    <row r="585" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A585" s="14"/>
+    </row>
+    <row r="586" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A586" s="14"/>
+    </row>
+    <row r="587" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A587" s="14"/>
+    </row>
+    <row r="588" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A588" s="14"/>
+    </row>
+    <row r="589" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A589" s="14"/>
+    </row>
+    <row r="590" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A590" s="14"/>
+    </row>
+    <row r="591" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A591" s="14"/>
+    </row>
+    <row r="592" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A592" s="14"/>
+    </row>
+    <row r="593" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A593" s="14"/>
+    </row>
+    <row r="594" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A594" s="14"/>
+    </row>
+    <row r="595" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A595" s="14"/>
+    </row>
+    <row r="596" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A596" s="14"/>
+    </row>
+    <row r="597" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A597" s="14"/>
+    </row>
+    <row r="598" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A598" s="14"/>
+    </row>
+    <row r="599" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A599" s="14"/>
+    </row>
+    <row r="600" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A600" s="14"/>
+    </row>
+    <row r="601" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A601" s="14"/>
+    </row>
+    <row r="602" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A602" s="14"/>
+    </row>
+    <row r="603" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A603" s="14"/>
+    </row>
+    <row r="604" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A604" s="14"/>
+    </row>
+    <row r="605" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A605" s="14"/>
+    </row>
+    <row r="606" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A606" s="14"/>
+    </row>
+    <row r="607" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A607" s="14"/>
+    </row>
+    <row r="608" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A608" s="14"/>
+    </row>
+    <row r="609" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A609" s="14"/>
+    </row>
+    <row r="610" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A610" s="14"/>
+    </row>
+    <row r="611" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A611" s="14"/>
+    </row>
+    <row r="612" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A612" s="14"/>
+    </row>
+    <row r="613" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A613" s="14"/>
+    </row>
+    <row r="614" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A614" s="14"/>
+    </row>
+    <row r="615" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A615" s="14"/>
+    </row>
+    <row r="616" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A616" s="14"/>
+    </row>
+    <row r="617" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A617" s="14"/>
+    </row>
+    <row r="618" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A618" s="14"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H426" xr:uid="{27C50DC2-CA37-49EF-A0FD-69B4D39A71AD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -11424,8 +10430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C0036E-3B56-45D0-8930-3C1E9E83B674}">
   <dimension ref="A1:D178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K96" sqref="K96"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D179" sqref="D179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12017,8 +11023,8 @@
       <c r="C42" s="26" t="s">
         <v>293</v>
       </c>
-      <c r="D42" s="26" t="s">
-        <v>294</v>
+      <c r="D42" s="26">
+        <v>171.84111709999999</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -12029,10 +11035,10 @@
         <v>126</v>
       </c>
       <c r="C43" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="D43" s="26" t="s">
         <v>295</v>
-      </c>
-      <c r="D43" s="26" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -12043,10 +11049,10 @@
         <v>127</v>
       </c>
       <c r="C44" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="D44" s="26" t="s">
         <v>297</v>
-      </c>
-      <c r="D44" s="26" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -12057,10 +11063,10 @@
         <v>128</v>
       </c>
       <c r="C45" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="D45" s="26" t="s">
         <v>299</v>
-      </c>
-      <c r="D45" s="26" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -12071,10 +11077,10 @@
         <v>129</v>
       </c>
       <c r="C46" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="D46" s="26" t="s">
         <v>301</v>
-      </c>
-      <c r="D46" s="26" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -12085,10 +11091,10 @@
         <v>130</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>303</v>
-      </c>
-      <c r="D47" s="26" t="s">
-        <v>304</v>
+        <v>302</v>
+      </c>
+      <c r="D47" s="26">
+        <v>171.76235</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -12099,10 +11105,10 @@
         <v>131</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -12113,10 +11119,10 @@
         <v>132</v>
       </c>
       <c r="C49" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -12127,10 +11133,10 @@
         <v>133</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -12141,10 +11147,10 @@
         <v>134</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -12155,10 +11161,10 @@
         <v>135</v>
       </c>
       <c r="C52" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="D52" s="26" t="s">
-        <v>314</v>
+        <v>311</v>
+      </c>
+      <c r="D52" s="26">
+        <v>171.61458999999999</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -12169,10 +11175,10 @@
         <v>136</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D53" s="26" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -12183,10 +11189,10 @@
         <v>137</v>
       </c>
       <c r="C54" s="26" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -12197,10 +11203,10 @@
         <v>138</v>
       </c>
       <c r="C55" s="26" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D55" s="26" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -12211,10 +11217,10 @@
         <v>139</v>
       </c>
       <c r="C56" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D56" s="26" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -12225,10 +11231,10 @@
         <v>140</v>
       </c>
       <c r="C57" s="26" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D57" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -12239,10 +11245,10 @@
         <v>141</v>
       </c>
       <c r="C58" s="26" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D58" s="26" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -12253,10 +11259,10 @@
         <v>142</v>
       </c>
       <c r="C59" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D59" s="26" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -12267,10 +11273,10 @@
         <v>143</v>
       </c>
       <c r="C60" s="26" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D60" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -12281,10 +11287,10 @@
         <v>144</v>
       </c>
       <c r="C61" s="26" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D61" s="26" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -12295,10 +11301,10 @@
         <v>145</v>
       </c>
       <c r="C62" s="26" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D62" s="26" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -12309,10 +11315,10 @@
         <v>146</v>
       </c>
       <c r="C63" s="26" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D63" s="26" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -12323,10 +11329,10 @@
         <v>147</v>
       </c>
       <c r="C64" s="26" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D64" s="26" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -12337,10 +11343,10 @@
         <v>148</v>
       </c>
       <c r="C65" s="26" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D65" s="26" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -12351,10 +11357,10 @@
         <v>149</v>
       </c>
       <c r="C66" s="26" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D66" s="26" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -12365,10 +11371,10 @@
         <v>150</v>
       </c>
       <c r="C67" s="26" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D67" s="26" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -12379,10 +11385,10 @@
         <v>151</v>
       </c>
       <c r="C68" s="26" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D68" s="26" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -12393,10 +11399,10 @@
         <v>152</v>
       </c>
       <c r="C69" s="26" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D69" s="26" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -12407,10 +11413,10 @@
         <v>153</v>
       </c>
       <c r="C70" s="26" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D70" s="26" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -12421,10 +11427,10 @@
         <v>154</v>
       </c>
       <c r="C71" s="26" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D71" s="26" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -12435,10 +11441,10 @@
         <v>155</v>
       </c>
       <c r="C72" s="26" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D72" s="26" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -12449,10 +11455,10 @@
         <v>156</v>
       </c>
       <c r="C73" s="26" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D73" s="26" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -12463,10 +11469,10 @@
         <v>157</v>
       </c>
       <c r="C74" s="26" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D74" s="26" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -12477,10 +11483,10 @@
         <v>158</v>
       </c>
       <c r="C75" s="26" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D75" s="26" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -12491,10 +11497,10 @@
         <v>159</v>
       </c>
       <c r="C76" s="26" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D76" s="26" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -12505,10 +11511,10 @@
         <v>160</v>
       </c>
       <c r="C77" s="26" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D77" s="26" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -12519,10 +11525,10 @@
         <v>161</v>
       </c>
       <c r="C78" s="26" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D78" s="26" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -12533,10 +11539,10 @@
         <v>162</v>
       </c>
       <c r="C79" s="26" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D79" s="26" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -12547,10 +11553,10 @@
         <v>163</v>
       </c>
       <c r="C80" s="26" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D80" s="26" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -12561,10 +11567,10 @@
         <v>164</v>
       </c>
       <c r="C81" s="26" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D81" s="26" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -12575,10 +11581,10 @@
         <v>165</v>
       </c>
       <c r="C82" s="26" t="s">
-        <v>373</v>
-      </c>
-      <c r="D82" s="26" t="s">
-        <v>374</v>
+        <v>370</v>
+      </c>
+      <c r="D82" s="26">
+        <v>171.6</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -12589,10 +11595,10 @@
         <v>166</v>
       </c>
       <c r="C83" s="26" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D83" s="26" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -12603,10 +11609,10 @@
         <v>167</v>
       </c>
       <c r="C84" s="26" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D84" s="26" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -12617,10 +11623,10 @@
         <v>168</v>
       </c>
       <c r="C85" s="26" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D85" s="26" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -12631,10 +11637,10 @@
         <v>169</v>
       </c>
       <c r="C86" s="26" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D86" s="26" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -12645,10 +11651,10 @@
         <v>170</v>
       </c>
       <c r="C87" s="26" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D87" s="26" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -12659,10 +11665,10 @@
         <v>171</v>
       </c>
       <c r="C88" s="26" t="s">
-        <v>385</v>
-      </c>
-      <c r="D88" s="26" t="s">
-        <v>386</v>
+        <v>381</v>
+      </c>
+      <c r="D88" s="26">
+        <v>171.41188</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -12673,10 +11679,10 @@
         <v>172</v>
       </c>
       <c r="C89" s="26" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="D89" s="26" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -12687,10 +11693,10 @@
         <v>173</v>
       </c>
       <c r="C90" s="26" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="D90" s="26" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -12701,10 +11707,10 @@
         <v>174</v>
       </c>
       <c r="C91" s="26" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="D91" s="26" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -12715,10 +11721,10 @@
         <v>175</v>
       </c>
       <c r="C92" s="26" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D92" s="26" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -12729,10 +11735,10 @@
         <v>176</v>
       </c>
       <c r="C93" s="26" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="D93" s="26" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -12743,7 +11749,7 @@
         <v>177</v>
       </c>
       <c r="C94" s="26" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="D94" s="26" t="s">
         <v>266</v>
@@ -12757,10 +11763,10 @@
         <v>178</v>
       </c>
       <c r="C95" s="26" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D95" s="26" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -12771,10 +11777,10 @@
         <v>179</v>
       </c>
       <c r="C96" s="26" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D96" s="26" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -12785,10 +11791,10 @@
         <v>180</v>
       </c>
       <c r="C97" s="26" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="D97" s="26" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -12799,10 +11805,10 @@
         <v>181</v>
       </c>
       <c r="C98" s="26" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="D98" s="26" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -12813,10 +11819,10 @@
         <v>182</v>
       </c>
       <c r="C99" s="26" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D99" s="26" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -12827,10 +11833,10 @@
         <v>183</v>
       </c>
       <c r="C100" s="26" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D100" s="26" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -12841,10 +11847,10 @@
         <v>184</v>
       </c>
       <c r="C101" s="26" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D101" s="26" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -12855,10 +11861,10 @@
         <v>185</v>
       </c>
       <c r="C102" s="26" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="D102" s="26" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -12869,10 +11875,10 @@
         <v>186</v>
       </c>
       <c r="C103" s="26" t="s">
-        <v>414</v>
-      </c>
-      <c r="D103" s="26" t="s">
-        <v>415</v>
+        <v>409</v>
+      </c>
+      <c r="D103" s="26">
+        <v>171.67816999999999</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -12883,10 +11889,10 @@
         <v>187</v>
       </c>
       <c r="C104" s="26" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="D104" s="26" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -12897,10 +11903,10 @@
         <v>188</v>
       </c>
       <c r="C105" s="26" t="s">
-        <v>418</v>
-      </c>
-      <c r="D105" s="26" t="s">
-        <v>419</v>
+        <v>412</v>
+      </c>
+      <c r="D105" s="26">
+        <v>171.62900999999999</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -12911,10 +11917,10 @@
         <v>189</v>
       </c>
       <c r="C106" s="26" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="D106" s="26" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -12925,10 +11931,10 @@
         <v>190</v>
       </c>
       <c r="C107" s="26" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="D107" s="26" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -12939,10 +11945,10 @@
         <v>191</v>
       </c>
       <c r="C108" s="26" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="D108" s="26" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -12953,10 +11959,10 @@
         <v>192</v>
       </c>
       <c r="C109" s="26" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="D109" s="26" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -12967,10 +11973,10 @@
         <v>193</v>
       </c>
       <c r="C110" s="26" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="D110" s="26" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -12981,10 +11987,10 @@
         <v>194</v>
       </c>
       <c r="C111" s="26" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="D111" s="26" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -12995,10 +12001,10 @@
         <v>195</v>
       </c>
       <c r="C112" s="26" t="s">
-        <v>432</v>
-      </c>
-      <c r="D112" s="26" t="s">
-        <v>433</v>
+        <v>425</v>
+      </c>
+      <c r="D112" s="26">
+        <v>171.53644</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -13009,10 +12015,10 @@
         <v>196</v>
       </c>
       <c r="C113" s="26" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="D113" s="26" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -13023,10 +12029,10 @@
         <v>197</v>
       </c>
       <c r="C114" s="26" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="D114" s="26" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -13037,10 +12043,10 @@
         <v>198</v>
       </c>
       <c r="C115" s="26" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="D115" s="26" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -13051,10 +12057,10 @@
         <v>199</v>
       </c>
       <c r="C116" s="26" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="D116" s="26" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -13065,10 +12071,10 @@
         <v>200</v>
       </c>
       <c r="C117" s="26" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="D117" s="26" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -13079,10 +12085,10 @@
         <v>201</v>
       </c>
       <c r="C118" s="26" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="D118" s="26" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -13093,10 +12099,10 @@
         <v>202</v>
       </c>
       <c r="C119" s="26" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="D119" s="26" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -13107,10 +12113,10 @@
         <v>203</v>
       </c>
       <c r="C120" s="26" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="D120" s="26" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -13121,10 +12127,10 @@
         <v>204</v>
       </c>
       <c r="C121" s="26" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="D121" s="26" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -13135,10 +12141,10 @@
         <v>205</v>
       </c>
       <c r="C122" s="26" t="s">
-        <v>452</v>
-      </c>
-      <c r="D122" s="26" t="s">
-        <v>453</v>
+        <v>444</v>
+      </c>
+      <c r="D122" s="26">
+        <v>171.70094</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -13149,10 +12155,10 @@
         <v>206</v>
       </c>
       <c r="C123" s="26" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="D123" s="26" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -13163,10 +12169,10 @@
         <v>207</v>
       </c>
       <c r="C124" s="26" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="D124" s="26" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -13177,10 +12183,10 @@
         <v>208</v>
       </c>
       <c r="C125" s="26" t="s">
-        <v>458</v>
-      </c>
-      <c r="D125" s="26" t="s">
-        <v>459</v>
+        <v>449</v>
+      </c>
+      <c r="D125" s="26">
+        <v>171.98658169999999</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -13191,10 +12197,10 @@
         <v>209</v>
       </c>
       <c r="C126" s="26" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="D126" s="26" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -13205,10 +12211,10 @@
         <v>210</v>
       </c>
       <c r="C127" s="26" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="D127" s="26" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -13219,10 +12225,10 @@
         <v>211</v>
       </c>
       <c r="C128" s="26" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="D128" s="26" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -13233,10 +12239,10 @@
         <v>212</v>
       </c>
       <c r="C129" s="26" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="D129" s="26" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -13247,10 +12253,10 @@
         <v>213</v>
       </c>
       <c r="C130" s="26" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="D130" s="26" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -13261,10 +12267,10 @@
         <v>214</v>
       </c>
       <c r="C131" s="26" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="D131" s="26" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -13275,10 +12281,10 @@
         <v>215</v>
       </c>
       <c r="C132" s="26" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
       <c r="D132" s="26" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -13289,10 +12295,10 @@
         <v>216</v>
       </c>
       <c r="C133" s="26" t="s">
-        <v>474</v>
+        <v>464</v>
       </c>
       <c r="D133" s="26" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -13303,10 +12309,10 @@
         <v>217</v>
       </c>
       <c r="C134" s="26" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="D134" s="26" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -13317,10 +12323,10 @@
         <v>217</v>
       </c>
       <c r="C135" s="26" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="D135" s="26" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -13331,10 +12337,10 @@
         <v>218</v>
       </c>
       <c r="C136" s="26" t="s">
-        <v>478</v>
+        <v>468</v>
       </c>
       <c r="D136" s="26" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -13345,10 +12351,10 @@
         <v>219</v>
       </c>
       <c r="C137" s="26" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
       <c r="D137" s="26" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -13359,10 +12365,10 @@
         <v>220</v>
       </c>
       <c r="C138" s="26" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="D138" s="26" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -13373,10 +12379,10 @@
         <v>221</v>
       </c>
       <c r="C139" s="26" t="s">
-        <v>484</v>
-      </c>
-      <c r="D139" s="26" t="s">
-        <v>485</v>
+        <v>474</v>
+      </c>
+      <c r="D139" s="26">
+        <v>172.10013000000001</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -13387,10 +12393,10 @@
         <v>222</v>
       </c>
       <c r="C140" s="26" t="s">
-        <v>486</v>
+        <v>475</v>
       </c>
       <c r="D140" s="26" t="s">
-        <v>487</v>
+        <v>476</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -13401,10 +12407,10 @@
         <v>223</v>
       </c>
       <c r="C141" s="26" t="s">
-        <v>488</v>
+        <v>477</v>
       </c>
       <c r="D141" s="26" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -13415,10 +12421,10 @@
         <v>224</v>
       </c>
       <c r="C142" s="26" t="s">
-        <v>490</v>
+        <v>479</v>
       </c>
       <c r="D142" s="26" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -13429,10 +12435,10 @@
         <v>225</v>
       </c>
       <c r="C143" s="26" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="D143" s="26" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -13443,10 +12449,10 @@
         <v>226</v>
       </c>
       <c r="C144" s="26" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
       <c r="D144" s="26" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -13457,10 +12463,10 @@
         <v>227</v>
       </c>
       <c r="C145" s="26" t="s">
-        <v>496</v>
+        <v>485</v>
       </c>
       <c r="D145" s="26" t="s">
-        <v>497</v>
+        <v>486</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -13471,10 +12477,10 @@
         <v>228</v>
       </c>
       <c r="C146" s="26" t="s">
-        <v>498</v>
+        <v>487</v>
       </c>
       <c r="D146" s="26" t="s">
-        <v>499</v>
+        <v>488</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -13485,10 +12491,10 @@
         <v>229</v>
       </c>
       <c r="C147" s="26" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="D147" s="26" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -13499,10 +12505,10 @@
         <v>230</v>
       </c>
       <c r="C148" s="26" t="s">
-        <v>502</v>
-      </c>
-      <c r="D148" s="26" t="s">
-        <v>503</v>
+        <v>491</v>
+      </c>
+      <c r="D148" s="26">
+        <v>171.72696999999999</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -13513,10 +12519,10 @@
         <v>231</v>
       </c>
       <c r="C149" s="26" t="s">
-        <v>504</v>
+        <v>492</v>
       </c>
       <c r="D149" s="26" t="s">
-        <v>505</v>
+        <v>493</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -13527,10 +12533,10 @@
         <v>232</v>
       </c>
       <c r="C150" s="26" t="s">
-        <v>506</v>
-      </c>
-      <c r="D150" s="26" t="s">
-        <v>507</v>
+        <v>494</v>
+      </c>
+      <c r="D150" s="26">
+        <v>171.93370999999999</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -13541,10 +12547,10 @@
         <v>233</v>
       </c>
       <c r="C151" s="26" t="s">
-        <v>508</v>
+        <v>495</v>
       </c>
       <c r="D151" s="26" t="s">
-        <v>509</v>
+        <v>496</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -13555,10 +12561,10 @@
         <v>234</v>
       </c>
       <c r="C152" s="26" t="s">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="D152" s="26" t="s">
-        <v>511</v>
+        <v>498</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -13569,10 +12575,10 @@
         <v>235</v>
       </c>
       <c r="C153" s="26" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="D153" s="26" t="s">
-        <v>513</v>
+        <v>500</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -13583,10 +12589,10 @@
         <v>236</v>
       </c>
       <c r="C154" s="26" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="D154" s="26" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -13597,10 +12603,10 @@
         <v>237</v>
       </c>
       <c r="C155" s="26" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="D155" s="26" t="s">
-        <v>517</v>
+        <v>504</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -13611,10 +12617,10 @@
         <v>238</v>
       </c>
       <c r="C156" s="26" t="s">
-        <v>518</v>
+        <v>505</v>
       </c>
       <c r="D156" s="26" t="s">
-        <v>519</v>
+        <v>506</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -13625,10 +12631,10 @@
         <v>239</v>
       </c>
       <c r="C157" s="26" t="s">
-        <v>520</v>
+        <v>507</v>
       </c>
       <c r="D157" s="26" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -13639,10 +12645,10 @@
         <v>240</v>
       </c>
       <c r="C158" s="26" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="D158" s="26" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -13653,10 +12659,10 @@
         <v>241</v>
       </c>
       <c r="C159" s="26" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
       <c r="D159" s="26" t="s">
-        <v>525</v>
+        <v>512</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -13667,10 +12673,10 @@
         <v>242</v>
       </c>
       <c r="C160" s="26" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
       <c r="D160" s="26" t="s">
-        <v>527</v>
+        <v>514</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -13681,10 +12687,10 @@
         <v>243</v>
       </c>
       <c r="C161" s="26" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="D161" s="26" t="s">
-        <v>529</v>
+        <v>516</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -13695,10 +12701,10 @@
         <v>244</v>
       </c>
       <c r="C162" s="26" t="s">
-        <v>530</v>
+        <v>517</v>
       </c>
       <c r="D162" s="26" t="s">
-        <v>531</v>
+        <v>518</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -13709,10 +12715,10 @@
         <v>245</v>
       </c>
       <c r="C163" s="26" t="s">
-        <v>532</v>
+        <v>519</v>
       </c>
       <c r="D163" s="26" t="s">
-        <v>533</v>
+        <v>520</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -13723,10 +12729,10 @@
         <v>246</v>
       </c>
       <c r="C164" s="26" t="s">
-        <v>534</v>
+        <v>521</v>
       </c>
       <c r="D164" s="26" t="s">
-        <v>535</v>
+        <v>522</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -13737,10 +12743,10 @@
         <v>247</v>
       </c>
       <c r="C165" s="26" t="s">
-        <v>536</v>
+        <v>523</v>
       </c>
       <c r="D165" s="26" t="s">
-        <v>537</v>
+        <v>524</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -13751,10 +12757,10 @@
         <v>248</v>
       </c>
       <c r="C166" s="26" t="s">
-        <v>538</v>
+        <v>525</v>
       </c>
       <c r="D166" s="26" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -13765,10 +12771,10 @@
         <v>249</v>
       </c>
       <c r="C167" s="26" t="s">
-        <v>540</v>
+        <v>527</v>
       </c>
       <c r="D167" s="26" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -13779,10 +12785,10 @@
         <v>250</v>
       </c>
       <c r="C168" s="26" t="s">
-        <v>542</v>
+        <v>529</v>
       </c>
       <c r="D168" s="26" t="s">
-        <v>543</v>
+        <v>530</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -13793,10 +12799,10 @@
         <v>251</v>
       </c>
       <c r="C169" s="26" t="s">
-        <v>544</v>
+        <v>531</v>
       </c>
       <c r="D169" s="26" t="s">
-        <v>545</v>
+        <v>532</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -13807,10 +12813,10 @@
         <v>252</v>
       </c>
       <c r="C170" s="26" t="s">
-        <v>546</v>
+        <v>533</v>
       </c>
       <c r="D170" s="26" t="s">
-        <v>547</v>
+        <v>534</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -13821,10 +12827,10 @@
         <v>253</v>
       </c>
       <c r="C171" s="26" t="s">
-        <v>548</v>
+        <v>535</v>
       </c>
       <c r="D171" s="26" t="s">
-        <v>549</v>
+        <v>536</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -13835,10 +12841,10 @@
         <v>254</v>
       </c>
       <c r="C172" s="26" t="s">
-        <v>550</v>
+        <v>537</v>
       </c>
       <c r="D172" s="26" t="s">
-        <v>551</v>
+        <v>538</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -13849,10 +12855,10 @@
         <v>255</v>
       </c>
       <c r="C173" s="26" t="s">
-        <v>552</v>
+        <v>539</v>
       </c>
       <c r="D173" s="26" t="s">
-        <v>553</v>
+        <v>540</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -13863,10 +12869,10 @@
         <v>256</v>
       </c>
       <c r="C174" s="26" t="s">
-        <v>554</v>
+        <v>541</v>
       </c>
       <c r="D174" s="26" t="s">
-        <v>555</v>
+        <v>542</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -13877,10 +12883,10 @@
         <v>257</v>
       </c>
       <c r="C175" s="26" t="s">
-        <v>556</v>
+        <v>543</v>
       </c>
       <c r="D175" s="26" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -13891,10 +12897,10 @@
         <v>258</v>
       </c>
       <c r="C176" s="26" t="s">
-        <v>558</v>
+        <v>545</v>
       </c>
       <c r="D176" s="26" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -13905,10 +12911,10 @@
         <v>259</v>
       </c>
       <c r="C177" s="26" t="s">
-        <v>560</v>
+        <v>547</v>
       </c>
       <c r="D177" s="26" t="s">
-        <v>561</v>
+        <v>548</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -13919,13 +12925,14 @@
         <v>260</v>
       </c>
       <c r="C178" s="26" t="s">
-        <v>562</v>
+        <v>549</v>
       </c>
       <c r="D178" s="26" t="s">
-        <v>563</v>
+        <v>550</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D178" xr:uid="{C0C0036E-3B56-45D0-8930-3C1E9E83B674}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added Hantz Honey data and reworked some bit and pieces from base R solution to dplyr solution
</commit_message>
<xml_diff>
--- a/data_in/Complete Mite Monitor GP.xlsx
+++ b/data_in/Complete Mite Monitor GP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GPetersen\Desktop\Mite_Monitor\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62DA990-E512-4EA6-A09E-35F4258DC25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEFB8C5-675E-4C18-97BF-30B66BAD41AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{16EEC1AB-7B5A-40BF-9CB7-5EB9EEF202EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{16EEC1AB-7B5A-40BF-9CB7-5EB9EEF202EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Mite Counts" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="613">
   <si>
     <t xml:space="preserve">TREATMENT
 </t>
@@ -1692,6 +1692,192 @@
   </si>
   <si>
     <t>171.722318</t>
+  </si>
+  <si>
+    <t>-43.871609, 171.883255</t>
+  </si>
+  <si>
+    <t>-43.87078, 171.824665</t>
+  </si>
+  <si>
+    <t>-43.770702, 172.018198</t>
+  </si>
+  <si>
+    <t>-43.78585, 172.001449</t>
+  </si>
+  <si>
+    <t>-43.886948, 172.051677</t>
+  </si>
+  <si>
+    <t>-43.885168, 171.958609</t>
+  </si>
+  <si>
+    <t>-43.876766, 172.166778</t>
+  </si>
+  <si>
+    <t>-43.911316, 171.849626</t>
+  </si>
+  <si>
+    <t>-43.816712, 172.101686</t>
+  </si>
+  <si>
+    <t>-43.77525, 172.05483</t>
+  </si>
+  <si>
+    <t>-43.899869, 171.937591</t>
+  </si>
+  <si>
+    <t>-43.87071, 172.14974</t>
+  </si>
+  <si>
+    <t>-43.883137, 172.092542</t>
+  </si>
+  <si>
+    <t>-43.895212, 172.131676</t>
+  </si>
+  <si>
+    <t>-43.729419, 171.863584</t>
+  </si>
+  <si>
+    <t>-43.705694, 171.826692</t>
+  </si>
+  <si>
+    <t>-43.681041, 171.766283</t>
+  </si>
+  <si>
+    <t>-43.753515, 171.884616</t>
+  </si>
+  <si>
+    <t>-43.700172, 171.89862</t>
+  </si>
+  <si>
+    <t>-43.69961, 171.90379</t>
+  </si>
+  <si>
+    <t>-43.83593, 171.70706</t>
+  </si>
+  <si>
+    <t>-43.77611, 171.91226</t>
+  </si>
+  <si>
+    <t>-43.62349, 171.78761</t>
+  </si>
+  <si>
+    <t>-43.63877, 171.80254</t>
+  </si>
+  <si>
+    <t>-43.68853, 171.81956</t>
+  </si>
+  <si>
+    <t>-43.76647, 171.93849</t>
+  </si>
+  <si>
+    <t>-43.78433, 172.21966</t>
+  </si>
+  <si>
+    <t>-43.782805, 172.196895</t>
+  </si>
+  <si>
+    <t>-43.7921, 172.23059</t>
+  </si>
+  <si>
+    <t>-43.817702, 172.247916</t>
+  </si>
+  <si>
+    <t>-43.85707, 172.286638</t>
+  </si>
+  <si>
+    <t>-43.844514, 172.307196</t>
+  </si>
+  <si>
+    <t>-43.700127, 172.216186</t>
+  </si>
+  <si>
+    <t>-43.873865, 172.241752</t>
+  </si>
+  <si>
+    <t>-43.72195, 172.18314</t>
+  </si>
+  <si>
+    <t>-43.813001, 172.182433</t>
+  </si>
+  <si>
+    <t>-43.816191, 172.262608</t>
+  </si>
+  <si>
+    <t>-43.681941, 172.189672</t>
+  </si>
+  <si>
+    <t>-43.803577, 172.209457</t>
+  </si>
+  <si>
+    <t>-43.820787, 172.240317</t>
+  </si>
+  <si>
+    <t>-43.85028, 172.3368</t>
+  </si>
+  <si>
+    <t>-43.805145, 172.183846</t>
+  </si>
+  <si>
+    <t>-43.771915, 172.21874</t>
+  </si>
+  <si>
+    <t>-43.647457, 172.202927</t>
+  </si>
+  <si>
+    <t>-43.692445, 172.343681</t>
+  </si>
+  <si>
+    <t>-43.725487, 172.376853</t>
+  </si>
+  <si>
+    <t>-43.693472, 172.358929</t>
+  </si>
+  <si>
+    <t>-43.78848, 172.312802</t>
+  </si>
+  <si>
+    <t>-43.718526, 172.287699</t>
+  </si>
+  <si>
+    <t>-43.728968, 172.363998</t>
+  </si>
+  <si>
+    <t>-43.715446, 172.37295</t>
+  </si>
+  <si>
+    <t>-43.60077, 172.4349</t>
+  </si>
+  <si>
+    <t>-43.742225, 172.272204</t>
+  </si>
+  <si>
+    <t>-43.701837, 172.227959</t>
+  </si>
+  <si>
+    <t>-43.761002, 172.262249</t>
+  </si>
+  <si>
+    <t>-43.73931, 172.23562</t>
+  </si>
+  <si>
+    <t>-43.649024, 172.19426</t>
+  </si>
+  <si>
+    <t>-43.735589, 172.522092</t>
+  </si>
+  <si>
+    <t>-43.59645, 172.413161</t>
+  </si>
+  <si>
+    <t>-43.732855, 172.390341</t>
+  </si>
+  <si>
+    <t>-43.64839, 172.232623</t>
+  </si>
+  <si>
+    <t>-43.665876, 172.440673</t>
   </si>
 </sst>
 </file>
@@ -1742,15 +1928,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1758,11 +1950,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1816,6 +2023,10 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2132,8 +2343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C50DC2-CA37-49EF-A0FD-69B4D39A71AD}">
   <dimension ref="A1:H618"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A541" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C357" sqref="C357:C360"/>
     </sheetView>
   </sheetViews>
@@ -10428,10 +10639,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C0036E-3B56-45D0-8930-3C1E9E83B674}">
-  <dimension ref="A1:D178"/>
+  <dimension ref="A1:D240"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D179" sqref="D179"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="D241" sqref="D241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12931,6 +13142,688 @@
         <v>550</v>
       </c>
     </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>96</v>
+      </c>
+      <c r="C179" s="28" t="s">
+        <v>551</v>
+      </c>
+      <c r="D179">
+        <v>171.88325499999999</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C180" s="28" t="s">
+        <v>552</v>
+      </c>
+      <c r="D180" s="27">
+        <v>171.82466500000001</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C181" s="28" t="s">
+        <v>553</v>
+      </c>
+      <c r="D181" s="27">
+        <v>172.01819800000001</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C182" s="28" t="s">
+        <v>554</v>
+      </c>
+      <c r="D182" s="27">
+        <v>172.00144900000001</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C183" s="28" t="s">
+        <v>555</v>
+      </c>
+      <c r="D183" s="27">
+        <v>172.05167700000001</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C184" s="28" t="s">
+        <v>556</v>
+      </c>
+      <c r="D184" s="27">
+        <v>171.958609</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C185" s="28" t="s">
+        <v>557</v>
+      </c>
+      <c r="D185" s="27">
+        <v>172.16677799999999</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C186" s="28" t="s">
+        <v>558</v>
+      </c>
+      <c r="D186" s="27">
+        <v>171.849626</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C187" s="28" t="s">
+        <v>559</v>
+      </c>
+      <c r="D187" s="27">
+        <v>172.101686</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C188" s="29" t="s">
+        <v>560</v>
+      </c>
+      <c r="D188" s="27">
+        <v>172.05483000000001</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C189" s="28" t="s">
+        <v>561</v>
+      </c>
+      <c r="D189" s="27">
+        <v>171.937591</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C190" s="28" t="s">
+        <v>562</v>
+      </c>
+      <c r="D190" s="27">
+        <v>172.14974000000001</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C191" s="28" t="s">
+        <v>563</v>
+      </c>
+      <c r="D191" s="27">
+        <v>172.09254200000001</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C192" s="28" t="s">
+        <v>564</v>
+      </c>
+      <c r="D192" s="27">
+        <v>172.131676</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C193" s="28" t="s">
+        <v>565</v>
+      </c>
+      <c r="D193" s="27">
+        <v>171.863584</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C194" s="28" t="s">
+        <v>566</v>
+      </c>
+      <c r="D194" s="27">
+        <v>171.82669200000001</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C195" s="28" t="s">
+        <v>567</v>
+      </c>
+      <c r="D195" s="27">
+        <v>171.76628299999999</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C196" s="28" t="s">
+        <v>568</v>
+      </c>
+      <c r="D196" s="27">
+        <v>171.88461599999999</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C197" s="28" t="s">
+        <v>569</v>
+      </c>
+      <c r="D197" s="27">
+        <v>171.89861999999999</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C198" s="28" t="s">
+        <v>570</v>
+      </c>
+      <c r="D198" s="27">
+        <v>171.90378999999999</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C199" s="28" t="s">
+        <v>571</v>
+      </c>
+      <c r="D199" s="27">
+        <v>171.70706000000001</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C200" s="28" t="s">
+        <v>572</v>
+      </c>
+      <c r="D200" s="27">
+        <v>171.91226</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C201" s="28" t="s">
+        <v>573</v>
+      </c>
+      <c r="D201" s="27">
+        <v>171.78761</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C202" s="28" t="s">
+        <v>574</v>
+      </c>
+      <c r="D202" s="27">
+        <v>171.80253999999999</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C203" s="28" t="s">
+        <v>575</v>
+      </c>
+      <c r="D203" s="27">
+        <v>171.81956</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C204" s="28" t="s">
+        <v>576</v>
+      </c>
+      <c r="D204" s="27">
+        <v>171.93849</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C205" s="28" t="s">
+        <v>577</v>
+      </c>
+      <c r="D205" s="27">
+        <v>172.21966</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C206" s="28" t="s">
+        <v>578</v>
+      </c>
+      <c r="D206" s="27">
+        <v>172.19689500000001</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C207" s="28" t="s">
+        <v>579</v>
+      </c>
+      <c r="D207" s="27">
+        <v>172.23059000000001</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C208" s="28" t="s">
+        <v>580</v>
+      </c>
+      <c r="D208" s="27">
+        <v>172.247916</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C209" s="28" t="s">
+        <v>581</v>
+      </c>
+      <c r="D209" s="27">
+        <v>172.28663800000001</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C210" s="28" t="s">
+        <v>582</v>
+      </c>
+      <c r="D210" s="27">
+        <v>172.307196</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C211" s="28" t="s">
+        <v>583</v>
+      </c>
+      <c r="D211" s="27">
+        <v>172.21618599999999</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C212" s="28" t="s">
+        <v>584</v>
+      </c>
+      <c r="D212" s="27">
+        <v>172.24175199999999</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C213" s="28" t="s">
+        <v>585</v>
+      </c>
+      <c r="D213" s="27">
+        <v>172.18314000000001</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C214" s="28" t="s">
+        <v>586</v>
+      </c>
+      <c r="D214" s="27">
+        <v>172.182433</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C215" s="28" t="s">
+        <v>587</v>
+      </c>
+      <c r="D215" s="27">
+        <v>172.262608</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C216" s="28" t="s">
+        <v>588</v>
+      </c>
+      <c r="D216" s="27">
+        <v>172.189672</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C217" s="28" t="s">
+        <v>589</v>
+      </c>
+      <c r="D217" s="27">
+        <v>172.20945699999999</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C218" s="28" t="s">
+        <v>590</v>
+      </c>
+      <c r="D218" s="27">
+        <v>172.240317</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C219" s="28" t="s">
+        <v>591</v>
+      </c>
+      <c r="D219" s="27">
+        <v>172.33680000000001</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C220" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="D220" s="27">
+        <v>172.18384599999999</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C221" s="28" t="s">
+        <v>593</v>
+      </c>
+      <c r="D221" s="27">
+        <v>172.21874</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C222" s="28" t="s">
+        <v>594</v>
+      </c>
+      <c r="D222" s="27">
+        <v>172.20292699999999</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C223" s="28" t="s">
+        <v>595</v>
+      </c>
+      <c r="D223" s="27">
+        <v>172.343681</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C224" s="28" t="s">
+        <v>596</v>
+      </c>
+      <c r="D224" s="27">
+        <v>172.37685300000001</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C225" s="28" t="s">
+        <v>597</v>
+      </c>
+      <c r="D225" s="27">
+        <v>172.35892899999999</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C226" s="28" t="s">
+        <v>598</v>
+      </c>
+      <c r="D226" s="27">
+        <v>172.312802</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C227" s="28" t="s">
+        <v>599</v>
+      </c>
+      <c r="D227" s="27">
+        <v>172.287699</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C228" s="28" t="s">
+        <v>600</v>
+      </c>
+      <c r="D228" s="27">
+        <v>172.36399800000001</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C229" s="29" t="s">
+        <v>601</v>
+      </c>
+      <c r="D229" s="27">
+        <v>172.37295</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C230" s="28" t="s">
+        <v>602</v>
+      </c>
+      <c r="D230" s="27">
+        <v>172.4349</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C231" s="28" t="s">
+        <v>603</v>
+      </c>
+      <c r="D231" s="27">
+        <v>172.27220399999999</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C232" s="28" t="s">
+        <v>604</v>
+      </c>
+      <c r="D232" s="27">
+        <v>172.227959</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C233" s="28" t="s">
+        <v>605</v>
+      </c>
+      <c r="D233" s="27">
+        <v>172.262249</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C234" s="28" t="s">
+        <v>606</v>
+      </c>
+      <c r="D234" s="27">
+        <v>172.23562000000001</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C235" s="28" t="s">
+        <v>607</v>
+      </c>
+      <c r="D235" s="27">
+        <v>172.19426000000001</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C236" s="30" t="s">
+        <v>608</v>
+      </c>
+      <c r="D236" s="27">
+        <v>172.52209199999999</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C237" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="D237" s="27">
+        <v>172.413161</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C238" s="28" t="s">
+        <v>610</v>
+      </c>
+      <c r="D238" s="27">
+        <v>172.39034100000001</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C239" s="28" t="s">
+        <v>611</v>
+      </c>
+      <c r="D239" s="27">
+        <v>172.23262299999999</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C240" s="28" t="s">
+        <v>612</v>
+      </c>
+      <c r="D240" s="27">
+        <v>172.440673</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D178" xr:uid="{C0C0036E-3B56-45D0-8930-3C1E9E83B674}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12938,6 +13831,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Excel" ma:contentTypeID="0x01010016D332592C8D48479BC5088ACC237C9F00F875CD2DA353744E902D1F8ECB7FB8F7" ma:contentTypeVersion="1" ma:contentTypeDescription="Abacus Excel" ma:contentTypeScope="" ma:versionID="9213e044986d295bc06b6756f65efeab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0283e241b5bf73c1e8e306c617ac2e5">
     <xsd:element name="properties">
@@ -13051,32 +13959,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00578B20-DBE6-4C1E-AA5B-AEA66F886039}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24B9C426-6A46-4884-8BF9-F2BB722B0DD4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -13091,15 +13983,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24B9C426-6A46-4884-8BF9-F2BB722B0DD4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00578B20-DBE6-4C1E-AA5B-AEA66F886039}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>